<commit_message>
Add Active diagram.vsd, Class diagram.vsd
</commit_message>
<xml_diff>
--- a/Риски.xlsx
+++ b/Риски.xlsx
@@ -466,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,69 +620,69 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="75">
-      <c r="A5" s="3">
+    <row r="25" spans="1:10" ht="75">
+      <c r="A25" s="3">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="2">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="H25" s="2">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="2">
-        <f>$H5*$I5</f>
+      <c r="J25" s="2">
+        <f>$H25*$I25</f>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45">
-      <c r="A6" s="3">
+    <row r="26" spans="1:10" ht="45">
+      <c r="A26" s="3">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="2">
-        <v>2</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="H26" s="2">
+        <v>2</v>
+      </c>
+      <c r="I26" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="2">
-        <f>$H6*$I6</f>
+      <c r="J26" s="2">
+        <f>$H26*$I26</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Интерфейс.vsd append, update Class diagram.vsd, update other files
</commit_message>
<xml_diff>
--- a/Риски.xlsx
+++ b/Риски.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -87,54 +87,63 @@
     <t>Сделать выговор, в случае сильно ущерба немного сократить финансирование или заменить плохо работающего на другого, если возможно</t>
   </si>
   <si>
-    <t>Окружение</t>
-  </si>
-  <si>
-    <t>Отключение электричества</t>
-  </si>
-  <si>
-    <t>Включить запасной генератор, если его нет официанты работают как до внедрения проекта</t>
-  </si>
-  <si>
-    <t>Установка запасного электрогенератора (предполагается, что он был до внедрения проекта)</t>
+    <t>Люди</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Уход из команды </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выяснить заранее, что и кого не устраивает. </t>
+  </si>
+  <si>
+    <t>Найти нового сотрудника.</t>
+  </si>
+  <si>
+    <t>Проект будет завершен не вовремя.</t>
+  </si>
+  <si>
+    <t>Периодически выполнять проверку системы</t>
+  </si>
+  <si>
+    <t>Вызвать специалиста</t>
+  </si>
+  <si>
+    <t>Проект выйдет из проектного расписания</t>
+  </si>
+  <si>
+    <t>Проблемы с интернетом</t>
+  </si>
+  <si>
+    <t>Пропал интернет</t>
+  </si>
+  <si>
+    <t>Уход сотрудника</t>
+  </si>
+  <si>
+    <t>Сломался компьютер разработчика</t>
   </si>
   <si>
     <t>Технические</t>
-  </si>
-  <si>
-    <t>Поломка оборудования</t>
-  </si>
-  <si>
-    <t>Сервер отключится, работа с клиентами временно прекратится</t>
-  </si>
-  <si>
-    <t>Прекращения работы ресторана</t>
-  </si>
-  <si>
-    <t>Ежемесячный тех-осмотр</t>
-  </si>
-  <si>
-    <t>Остановка работы, проведение технических работ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <shadow/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -156,20 +165,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -466,14 +479,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
@@ -483,7 +497,9 @@
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.140625"/>
     <col min="12" max="12" width="34.7109375" customWidth="1"/>
+    <col min="13" max="256" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -519,35 +535,35 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="90">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2">
-        <f>$H2*$I2</f>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J7" si="0">$H2*$I2</f>
         <v>4</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -555,140 +571,172 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="90">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="2">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3">
         <v>3</v>
       </c>
-      <c r="J3" s="2">
-        <f>$H3*$I3</f>
+      <c r="J3" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="120">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2">
-        <v>2</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
         <v>3</v>
       </c>
-      <c r="J4" s="2">
-        <f>$H4*$I4</f>
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="75">
-      <c r="A25" s="3">
+    <row r="5" spans="1:12" ht="45">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="2">
-        <v>2</v>
-      </c>
-      <c r="I25" s="2">
-        <v>1</v>
-      </c>
-      <c r="J25" s="2">
-        <f>$H25*$I25</f>
-        <v>2</v>
+      <c r="G6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="45">
-      <c r="A26" s="3">
+    <row r="7" spans="1:12" ht="45">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="2">
-        <v>2</v>
-      </c>
-      <c r="I26" s="2">
-        <v>1</v>
-      </c>
-      <c r="J26" s="2">
-        <f>$H26*$I26</f>
-        <v>2</v>
+      <c r="H7" s="3">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>